<commit_message>
Reports for Inquiry API
</commit_message>
<xml_diff>
--- a/accums-service/src/test/resources/jmeter/report/ClaimUtilization_BenefitBalance_Inquiry_Report.xlsx
+++ b/accums-service/src/test/resources/jmeter/report/ClaimUtilization_BenefitBalance_Inquiry_Report.xlsx
@@ -4,10 +4,13 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="V1" sheetId="2" r:id="rId1"/>
+    <sheet name="V2" sheetId="3" r:id="rId2"/>
+    <sheet name="V3" sheetId="4" r:id="rId3"/>
+    <sheet name="V4" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913" calcOnSave="0"/>
   <extLst>
@@ -19,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="26">
   <si>
     <t>Label</t>
   </si>
@@ -96,7 +99,7 @@
     <t>Records - Before Inquiry</t>
   </si>
   <si>
-    <t>BASPIKES 10 with member ID</t>
+    <t>Accums Ledger Inquiry Performance Test:BASPIKES 10 with member ID</t>
   </si>
 </sst>
 </file>
@@ -212,55 +215,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>232966</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>281383</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>52386</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="232966" y="2406650"/>
-          <a:ext cx="9630567" cy="5011736"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -528,8 +482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -614,7 +568,7 @@
         <v>21</v>
       </c>
       <c r="O2" s="4">
-        <v>332757</v>
+        <v>332896</v>
       </c>
       <c r="P2" s="4" t="s">
         <v>20</v>
@@ -628,37 +582,37 @@
         <v>100</v>
       </c>
       <c r="C3">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="D3">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E3">
-        <v>876</v>
+        <v>226</v>
       </c>
       <c r="F3">
-        <v>149.75</v>
+        <v>46.22</v>
       </c>
       <c r="G3" s="1">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="H3">
-        <v>62.111800000000002</v>
+        <v>69.930070000000001</v>
       </c>
       <c r="I3">
-        <v>77.73</v>
+        <v>87.07</v>
       </c>
       <c r="J3">
-        <v>9.93</v>
+        <v>12.5</v>
       </c>
       <c r="K3">
-        <v>1281.5</v>
+        <v>1275</v>
       </c>
       <c r="N3" s="4" t="s">
         <v>22</v>
       </c>
       <c r="O3" s="4">
-        <v>1654169</v>
+        <v>1654843</v>
       </c>
       <c r="P3" s="4" t="s">
         <v>20</v>
@@ -672,37 +626,37 @@
         <v>100</v>
       </c>
       <c r="C4">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="D4">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E4">
-        <v>876</v>
+        <v>226</v>
       </c>
       <c r="F4">
-        <v>149.75</v>
+        <v>46.22</v>
       </c>
       <c r="G4" s="1">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="H4">
-        <v>62.111800000000002</v>
+        <v>69.930070000000001</v>
       </c>
       <c r="I4">
-        <v>77.73</v>
+        <v>87.07</v>
       </c>
       <c r="J4">
-        <v>9.93</v>
+        <v>12.5</v>
       </c>
       <c r="K4">
-        <v>1281.5</v>
+        <v>1275</v>
       </c>
       <c r="N4" s="4" t="s">
         <v>23</v>
       </c>
       <c r="O4" s="4">
-        <v>1402567</v>
+        <v>1403207</v>
       </c>
       <c r="P4" s="4" t="s">
         <v>20</v>
@@ -781,37 +735,37 @@
         <v>100</v>
       </c>
       <c r="C10">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="D10">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="E10">
-        <v>230</v>
+        <v>44</v>
       </c>
       <c r="F10">
-        <v>436</v>
+        <v>181</v>
       </c>
       <c r="G10">
-        <v>633</v>
+        <v>201</v>
       </c>
       <c r="H10">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="I10">
-        <v>876</v>
+        <v>226</v>
       </c>
       <c r="J10" s="1">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="K10">
-        <v>62.111800000000002</v>
+        <v>69.930070000000001</v>
       </c>
       <c r="L10">
-        <v>77.73</v>
+        <v>87.07</v>
       </c>
       <c r="M10">
-        <v>9.93</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.35">
@@ -822,37 +776,37 @@
         <v>100</v>
       </c>
       <c r="C11">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="D11">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="E11">
-        <v>230</v>
+        <v>44</v>
       </c>
       <c r="F11">
-        <v>436</v>
+        <v>181</v>
       </c>
       <c r="G11">
-        <v>633</v>
+        <v>201</v>
       </c>
       <c r="H11">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="I11">
-        <v>876</v>
+        <v>226</v>
       </c>
       <c r="J11" s="1">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="K11">
-        <v>62.111800000000002</v>
+        <v>69.930070000000001</v>
       </c>
       <c r="L11">
-        <v>77.73</v>
+        <v>87.07</v>
       </c>
       <c r="M11">
-        <v>9.93</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.35">
@@ -883,6 +837,1088 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.08984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.81640625" customWidth="1"/>
+    <col min="9" max="9" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.81640625" customWidth="1"/>
+    <col min="12" max="12" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.90625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.1796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="P1" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" t="s">
+        <v>15</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="O2" s="4">
+        <v>332896</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3">
+        <v>400</v>
+      </c>
+      <c r="C3">
+        <v>193</v>
+      </c>
+      <c r="D3">
+        <v>5</v>
+      </c>
+      <c r="E3">
+        <v>2308</v>
+      </c>
+      <c r="F3">
+        <v>391.1</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>62.46096</v>
+      </c>
+      <c r="I3">
+        <v>77.77</v>
+      </c>
+      <c r="J3">
+        <v>11.16</v>
+      </c>
+      <c r="K3">
+        <v>1275</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="O3" s="4">
+        <v>1654843</v>
+      </c>
+      <c r="P3" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4">
+        <v>400</v>
+      </c>
+      <c r="C4">
+        <v>193</v>
+      </c>
+      <c r="D4">
+        <v>5</v>
+      </c>
+      <c r="E4">
+        <v>2308</v>
+      </c>
+      <c r="F4">
+        <v>391.1</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>62.46096</v>
+      </c>
+      <c r="I4">
+        <v>77.77</v>
+      </c>
+      <c r="J4">
+        <v>11.16</v>
+      </c>
+      <c r="K4">
+        <v>1275</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="O4" s="4">
+        <v>1403207</v>
+      </c>
+      <c r="P4" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="G6" s="1"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A8" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" t="s">
+        <v>5</v>
+      </c>
+      <c r="G9" t="s">
+        <v>6</v>
+      </c>
+      <c r="H9" t="s">
+        <v>7</v>
+      </c>
+      <c r="I9" t="s">
+        <v>8</v>
+      </c>
+      <c r="J9" t="s">
+        <v>9</v>
+      </c>
+      <c r="K9" t="s">
+        <v>10</v>
+      </c>
+      <c r="L9" t="s">
+        <v>11</v>
+      </c>
+      <c r="M9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10">
+        <v>400</v>
+      </c>
+      <c r="C10">
+        <v>193</v>
+      </c>
+      <c r="D10">
+        <v>37</v>
+      </c>
+      <c r="E10">
+        <v>559</v>
+      </c>
+      <c r="F10">
+        <v>1412</v>
+      </c>
+      <c r="G10">
+        <v>1876</v>
+      </c>
+      <c r="H10">
+        <v>5</v>
+      </c>
+      <c r="I10">
+        <v>2308</v>
+      </c>
+      <c r="J10" s="1">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>62.46096</v>
+      </c>
+      <c r="L10">
+        <v>77.77</v>
+      </c>
+      <c r="M10">
+        <v>11.16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11">
+        <v>400</v>
+      </c>
+      <c r="C11">
+        <v>193</v>
+      </c>
+      <c r="D11">
+        <v>37</v>
+      </c>
+      <c r="E11">
+        <v>559</v>
+      </c>
+      <c r="F11">
+        <v>1412</v>
+      </c>
+      <c r="G11">
+        <v>1876</v>
+      </c>
+      <c r="H11">
+        <v>5</v>
+      </c>
+      <c r="I11">
+        <v>2308</v>
+      </c>
+      <c r="J11" s="1">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>62.46096</v>
+      </c>
+      <c r="L11">
+        <v>77.77</v>
+      </c>
+      <c r="M11">
+        <v>11.16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="J12" s="1"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="J13" s="1"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="J14" s="1"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="J15" s="1"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="J16" s="1"/>
+    </row>
+    <row r="17" spans="10:10" x14ac:dyDescent="0.35">
+      <c r="J17" s="1"/>
+    </row>
+    <row r="18" spans="10:10" x14ac:dyDescent="0.35">
+      <c r="J18" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A8:N8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E20" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.08984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.81640625" customWidth="1"/>
+    <col min="9" max="9" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.81640625" customWidth="1"/>
+    <col min="12" max="12" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.90625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.1796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="P1" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" t="s">
+        <v>15</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="O2" s="4">
+        <v>332896</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3">
+        <v>1600</v>
+      </c>
+      <c r="C3">
+        <v>633</v>
+      </c>
+      <c r="D3">
+        <v>5</v>
+      </c>
+      <c r="E3">
+        <v>2518</v>
+      </c>
+      <c r="F3">
+        <v>732.61</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>54.41066</v>
+      </c>
+      <c r="I3">
+        <v>67.75</v>
+      </c>
+      <c r="J3">
+        <v>9.7200000000000006</v>
+      </c>
+      <c r="K3">
+        <v>1275</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="O3" s="4">
+        <v>1654843</v>
+      </c>
+      <c r="P3" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4">
+        <v>1600</v>
+      </c>
+      <c r="C4">
+        <v>633</v>
+      </c>
+      <c r="D4">
+        <v>5</v>
+      </c>
+      <c r="E4">
+        <v>2518</v>
+      </c>
+      <c r="F4">
+        <v>732.61</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>54.41066</v>
+      </c>
+      <c r="I4">
+        <v>67.75</v>
+      </c>
+      <c r="J4">
+        <v>9.7200000000000006</v>
+      </c>
+      <c r="K4">
+        <v>1275</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="O4" s="4">
+        <v>1403207</v>
+      </c>
+      <c r="P4" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="G6" s="1"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A8" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" t="s">
+        <v>5</v>
+      </c>
+      <c r="G9" t="s">
+        <v>6</v>
+      </c>
+      <c r="H9" t="s">
+        <v>7</v>
+      </c>
+      <c r="I9" t="s">
+        <v>8</v>
+      </c>
+      <c r="J9" t="s">
+        <v>9</v>
+      </c>
+      <c r="K9" t="s">
+        <v>10</v>
+      </c>
+      <c r="L9" t="s">
+        <v>11</v>
+      </c>
+      <c r="M9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10">
+        <v>1600</v>
+      </c>
+      <c r="C10">
+        <v>633</v>
+      </c>
+      <c r="D10">
+        <v>265</v>
+      </c>
+      <c r="E10">
+        <v>1819</v>
+      </c>
+      <c r="F10">
+        <v>2122</v>
+      </c>
+      <c r="G10">
+        <v>2354</v>
+      </c>
+      <c r="H10">
+        <v>5</v>
+      </c>
+      <c r="I10">
+        <v>2518</v>
+      </c>
+      <c r="J10" s="1">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>54.41066</v>
+      </c>
+      <c r="L10">
+        <v>67.75</v>
+      </c>
+      <c r="M10">
+        <v>9.7200000000000006</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11">
+        <v>1600</v>
+      </c>
+      <c r="C11">
+        <v>633</v>
+      </c>
+      <c r="D11">
+        <v>265</v>
+      </c>
+      <c r="E11">
+        <v>1819</v>
+      </c>
+      <c r="F11">
+        <v>2122</v>
+      </c>
+      <c r="G11">
+        <v>2354</v>
+      </c>
+      <c r="H11">
+        <v>5</v>
+      </c>
+      <c r="I11">
+        <v>2518</v>
+      </c>
+      <c r="J11" s="1">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>54.41066</v>
+      </c>
+      <c r="L11">
+        <v>67.75</v>
+      </c>
+      <c r="M11">
+        <v>9.7200000000000006</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="J12" s="1"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="J13" s="1"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="J14" s="1"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="J15" s="1"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="J16" s="1"/>
+    </row>
+    <row r="17" spans="10:10" x14ac:dyDescent="0.35">
+      <c r="J17" s="1"/>
+    </row>
+    <row r="18" spans="10:10" x14ac:dyDescent="0.35">
+      <c r="J18" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A8:N8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:L1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.08984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.81640625" customWidth="1"/>
+    <col min="9" max="9" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.81640625" customWidth="1"/>
+    <col min="12" max="12" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.90625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.1796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="P1" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" t="s">
+        <v>15</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="O2" s="4">
+        <v>332896</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3">
+        <v>3600</v>
+      </c>
+      <c r="C3">
+        <v>1304</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>3830</v>
+      </c>
+      <c r="F3">
+        <v>1059</v>
+      </c>
+      <c r="G3" s="1">
+        <v>2.7999999999999998E-4</v>
+      </c>
+      <c r="H3">
+        <v>43.411679999999997</v>
+      </c>
+      <c r="I3">
+        <v>54.05</v>
+      </c>
+      <c r="J3">
+        <v>7.76</v>
+      </c>
+      <c r="K3">
+        <v>1275</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="O3" s="4">
+        <v>1654843</v>
+      </c>
+      <c r="P3" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4">
+        <v>3600</v>
+      </c>
+      <c r="C4">
+        <v>1304</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>3830</v>
+      </c>
+      <c r="F4">
+        <v>1059</v>
+      </c>
+      <c r="G4" s="1">
+        <v>2.7999999999999998E-4</v>
+      </c>
+      <c r="H4">
+        <v>43.411679999999997</v>
+      </c>
+      <c r="I4">
+        <v>54.05</v>
+      </c>
+      <c r="J4">
+        <v>7.76</v>
+      </c>
+      <c r="K4">
+        <v>1275</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="O4" s="4">
+        <v>1403207</v>
+      </c>
+      <c r="P4" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="G6" s="1"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A8" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" t="s">
+        <v>5</v>
+      </c>
+      <c r="G9" t="s">
+        <v>6</v>
+      </c>
+      <c r="H9" t="s">
+        <v>7</v>
+      </c>
+      <c r="I9" t="s">
+        <v>8</v>
+      </c>
+      <c r="J9" t="s">
+        <v>9</v>
+      </c>
+      <c r="K9" t="s">
+        <v>10</v>
+      </c>
+      <c r="L9" t="s">
+        <v>11</v>
+      </c>
+      <c r="M9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10">
+        <v>3600</v>
+      </c>
+      <c r="C10">
+        <v>1304</v>
+      </c>
+      <c r="D10">
+        <v>778</v>
+      </c>
+      <c r="E10">
+        <v>2811</v>
+      </c>
+      <c r="F10">
+        <v>3016</v>
+      </c>
+      <c r="G10">
+        <v>3407</v>
+      </c>
+      <c r="H10">
+        <v>3</v>
+      </c>
+      <c r="I10">
+        <v>3830</v>
+      </c>
+      <c r="J10" s="1">
+        <v>2.7999999999999998E-4</v>
+      </c>
+      <c r="K10">
+        <v>43.411679999999997</v>
+      </c>
+      <c r="L10">
+        <v>54.05</v>
+      </c>
+      <c r="M10">
+        <v>7.76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11">
+        <v>3600</v>
+      </c>
+      <c r="C11">
+        <v>1304</v>
+      </c>
+      <c r="D11">
+        <v>778</v>
+      </c>
+      <c r="E11">
+        <v>2811</v>
+      </c>
+      <c r="F11">
+        <v>3016</v>
+      </c>
+      <c r="G11">
+        <v>3407</v>
+      </c>
+      <c r="H11">
+        <v>3</v>
+      </c>
+      <c r="I11">
+        <v>3830</v>
+      </c>
+      <c r="J11" s="1">
+        <v>2.7999999999999998E-4</v>
+      </c>
+      <c r="K11">
+        <v>43.411679999999997</v>
+      </c>
+      <c r="L11">
+        <v>54.05</v>
+      </c>
+      <c r="M11">
+        <v>7.76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="J12" s="1"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="J13" s="1"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="J14" s="1"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="J15" s="1"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="J16" s="1"/>
+    </row>
+    <row r="17" spans="10:10" x14ac:dyDescent="0.35">
+      <c r="J17" s="1"/>
+    </row>
+    <row r="18" spans="10:10" x14ac:dyDescent="0.35">
+      <c r="J18" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A8:N8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Request/sec field in reports
</commit_message>
<xml_diff>
--- a/accums-service/src/test/resources/jmeter/report/ClaimUtilization_BenefitBalance_Inquiry_Report.xlsx
+++ b/accums-service/src/test/resources/jmeter/report/ClaimUtilization_BenefitBalance_Inquiry_Report.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
   </bookViews>
   <sheets>
     <sheet name="V1" sheetId="2" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="27">
   <si>
     <t>Label</t>
   </si>
@@ -100,6 +100,9 @@
   </si>
   <si>
     <t>Accums Ledger Inquiry Performance Test:BASPIKES 10 with member ID</t>
+  </si>
+  <si>
+    <t>Request/sec</t>
   </si>
 </sst>
 </file>
@@ -482,8 +485,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -564,6 +567,9 @@
       <c r="K2" t="s">
         <v>15</v>
       </c>
+      <c r="L2" t="s">
+        <v>26</v>
+      </c>
       <c r="N2" s="4" t="s">
         <v>21</v>
       </c>
@@ -608,6 +614,10 @@
       <c r="K3">
         <v>1275</v>
       </c>
+      <c r="L3">
+        <f>H3*60</f>
+        <v>4195.8042000000005</v>
+      </c>
       <c r="N3" s="4" t="s">
         <v>22</v>
       </c>
@@ -651,6 +661,10 @@
       </c>
       <c r="K4">
         <v>1275</v>
+      </c>
+      <c r="L4">
+        <f>H4*60</f>
+        <v>4195.8042000000005</v>
       </c>
       <c r="N4" s="4" t="s">
         <v>23</v>
@@ -726,6 +740,9 @@
       <c r="M9" t="s">
         <v>12</v>
       </c>
+      <c r="N9" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
@@ -767,6 +784,10 @@
       <c r="M10">
         <v>12.5</v>
       </c>
+      <c r="N10">
+        <f>K10*60</f>
+        <v>4195.8042000000005</v>
+      </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
@@ -807,6 +828,10 @@
       </c>
       <c r="M11">
         <v>12.5</v>
+      </c>
+      <c r="N11">
+        <f>K11*60</f>
+        <v>4195.8042000000005</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.35">
@@ -845,7 +870,7 @@
   <dimension ref="A1:P18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="A1:XFD1048576"/>
+      <selection activeCell="L2" sqref="L2:L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -926,6 +951,9 @@
       <c r="K2" t="s">
         <v>15</v>
       </c>
+      <c r="L2" t="s">
+        <v>26</v>
+      </c>
       <c r="N2" s="4" t="s">
         <v>21</v>
       </c>
@@ -970,6 +998,10 @@
       <c r="K3">
         <v>1275</v>
       </c>
+      <c r="L3">
+        <f>H3*60</f>
+        <v>3747.6576</v>
+      </c>
       <c r="N3" s="4" t="s">
         <v>22</v>
       </c>
@@ -1013,6 +1045,10 @@
       </c>
       <c r="K4">
         <v>1275</v>
+      </c>
+      <c r="L4">
+        <f>H4*60</f>
+        <v>3747.6576</v>
       </c>
       <c r="N4" s="4" t="s">
         <v>23</v>
@@ -1088,6 +1124,9 @@
       <c r="M9" t="s">
         <v>12</v>
       </c>
+      <c r="N9" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
@@ -1129,6 +1168,10 @@
       <c r="M10">
         <v>11.16</v>
       </c>
+      <c r="N10">
+        <f>K10*60</f>
+        <v>3747.6576</v>
+      </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
@@ -1169,6 +1212,10 @@
       </c>
       <c r="M11">
         <v>11.16</v>
+      </c>
+      <c r="N11">
+        <f>K11*60</f>
+        <v>3747.6576</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.35">
@@ -1206,7 +1253,7 @@
   <dimension ref="A1:P18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="A1:XFD1048576"/>
+      <selection activeCell="L2" sqref="L2:L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1287,6 +1334,9 @@
       <c r="K2" t="s">
         <v>15</v>
       </c>
+      <c r="L2" t="s">
+        <v>26</v>
+      </c>
       <c r="N2" s="4" t="s">
         <v>21</v>
       </c>
@@ -1331,6 +1381,10 @@
       <c r="K3">
         <v>1275</v>
       </c>
+      <c r="L3">
+        <f>H3*60</f>
+        <v>3264.6396</v>
+      </c>
       <c r="N3" s="4" t="s">
         <v>22</v>
       </c>
@@ -1374,6 +1428,10 @@
       </c>
       <c r="K4">
         <v>1275</v>
+      </c>
+      <c r="L4">
+        <f>H4*60</f>
+        <v>3264.6396</v>
       </c>
       <c r="N4" s="4" t="s">
         <v>23</v>
@@ -1449,6 +1507,9 @@
       <c r="M9" t="s">
         <v>12</v>
       </c>
+      <c r="N9" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
@@ -1490,6 +1551,10 @@
       <c r="M10">
         <v>9.7200000000000006</v>
       </c>
+      <c r="N10">
+        <f>K10*60</f>
+        <v>3264.6396</v>
+      </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
@@ -1530,6 +1595,10 @@
       </c>
       <c r="M11">
         <v>9.7200000000000006</v>
+      </c>
+      <c r="N11">
+        <f>K11*60</f>
+        <v>3264.6396</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.35">
@@ -1566,8 +1635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:L1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1648,6 +1717,9 @@
       <c r="K2" t="s">
         <v>15</v>
       </c>
+      <c r="L2" t="s">
+        <v>26</v>
+      </c>
       <c r="N2" s="4" t="s">
         <v>21</v>
       </c>
@@ -1692,6 +1764,10 @@
       <c r="K3">
         <v>1275</v>
       </c>
+      <c r="L3">
+        <f>H3*60</f>
+        <v>2604.7007999999996</v>
+      </c>
       <c r="N3" s="4" t="s">
         <v>22</v>
       </c>
@@ -1735,6 +1811,10 @@
       </c>
       <c r="K4">
         <v>1275</v>
+      </c>
+      <c r="L4">
+        <f>H4*60</f>
+        <v>2604.7007999999996</v>
       </c>
       <c r="N4" s="4" t="s">
         <v>23</v>
@@ -1810,6 +1890,9 @@
       <c r="M9" t="s">
         <v>12</v>
       </c>
+      <c r="N9" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
@@ -1851,6 +1934,10 @@
       <c r="M10">
         <v>7.76</v>
       </c>
+      <c r="N10">
+        <f>K10*60</f>
+        <v>2604.7007999999996</v>
+      </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
@@ -1891,6 +1978,10 @@
       </c>
       <c r="M11">
         <v>7.76</v>
+      </c>
+      <c r="N11">
+        <f>K11*60</f>
+        <v>2604.7007999999996</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.35">

</xml_diff>